<commit_message>
Improvements - Added ItestListner.
</commit_message>
<xml_diff>
--- a/MasterSheet.xlsx
+++ b/MasterSheet.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24360" windowHeight="10695"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="1" r:id="rId1"/>
     <sheet name="ResultSheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="77">
   <si>
     <t>TestScript Name</t>
   </si>
@@ -246,16 +247,13 @@
   </si>
   <si>
     <t>googlechrome</t>
-  </si>
-  <si>
-    <t>https://cscvsrdnor001.fsg.amer.csc.com/loginsp14j/secbypass.aspx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,14 +273,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,12 +310,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -340,12 +329,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,7 +638,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,13 +667,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -699,7 +686,7 @@
       <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>75</v>
       </c>
     </row>
@@ -730,7 +717,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,9 +1211,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>